<commit_message>
Dicionário de dados atualizado
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcmma\Documents\GitHub\BD_Faculdade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Napp - Integração\Documents\GitHub\BD_Faculdade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823FAAD5-0E28-4AC3-86EF-D778ACA72244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58624865-CC14-4B79-9C21-C458C4D953BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{7322636D-572D-48CD-9664-CDD954481AED}"/>
+    <workbookView xWindow="-21720" yWindow="-1185" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{7322636D-572D-48CD-9664-CDD954481AED}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="162">
   <si>
     <t>DICIONÁRIO DE DADOS: ENTIDADES</t>
   </si>
@@ -516,7 +516,10 @@
     <t>2ªFORMA NORMAL</t>
   </si>
   <si>
-    <t>Verificar se todos os atributos não-chave são dependentes da chave primária. (Não pode haver dependências parciais)</t>
+    <t>Verificar se todos os atributos não-chave são fucnionalmente dependentes da chave primária. Não pode haver dependências parciais. Atributos não dependem de chaves candidatas.</t>
+  </si>
+  <si>
+    <t>2ª Forma Normal aplicada</t>
   </si>
 </sst>
 </file>
@@ -877,73 +880,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -952,14 +889,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1281,27 +1284,27 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="31.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+    <row r="1" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1315,14 +1318,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1331,32 +1334,32 @@
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="D8" s="36"/>
+    </row>
+    <row r="9" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1365,22 +1368,22 @@
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
+    <row r="10" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="D10" s="36"/>
+    </row>
+    <row r="11" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1389,22 +1392,22 @@
       <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
+    <row r="12" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="D12" s="36"/>
+    </row>
+    <row r="13" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1413,42 +1416,42 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
+    <row r="14" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
       <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
       <c r="B15" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39"/>
       <c r="B16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -1457,42 +1460,42 @@
       <c r="C17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
+    <row r="18" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
       <c r="B18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
       <c r="B19" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
       <c r="B20" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -1501,62 +1504,62 @@
       <c r="C21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
+    <row r="22" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
       <c r="B22" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="28"/>
-    </row>
-    <row r="23" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
       <c r="B23" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="28"/>
-    </row>
-    <row r="24" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
       <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="28"/>
-    </row>
-    <row r="25" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="25" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="28"/>
-    </row>
-    <row r="26" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
       <c r="B26" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="D26" s="36"/>
+    </row>
+    <row r="27" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="16" t="s">
@@ -1565,22 +1568,22 @@
       <c r="C27" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
+    <row r="28" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="33"/>
       <c r="B28" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="27"/>
-    </row>
-    <row r="29" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
+      <c r="D28" s="36"/>
+    </row>
+    <row r="29" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -1589,22 +1592,22 @@
       <c r="C29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
+    <row r="30" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="33"/>
       <c r="B30" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="27"/>
-    </row>
-    <row r="31" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="D30" s="36"/>
+    </row>
+    <row r="31" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="16" t="s">
@@ -1613,22 +1616,22 @@
       <c r="C31" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
+    <row r="32" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="33"/>
       <c r="B32" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="D32" s="36"/>
+    </row>
+    <row r="33" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="16" t="s">
@@ -1637,22 +1640,22 @@
       <c r="C33" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
+    <row r="34" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="33"/>
       <c r="B34" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="27"/>
-    </row>
-    <row r="35" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
+      <c r="D34" s="36"/>
+    </row>
+    <row r="35" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="16" t="s">
@@ -1661,38 +1664,22 @@
       <c r="C35" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="25"/>
+    <row r="36" spans="1:4" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="33"/>
       <c r="B36" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="27"/>
+      <c r="D36" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="D29:D30"/>
@@ -1700,6 +1687,22 @@
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1708,62 +1711,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0621C709-D833-4B1E-A869-0A41CA3D9B62}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+    <row r="1" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-    </row>
-    <row r="3" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+    </row>
+    <row r="3" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="H4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="J4" s="27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
@@ -1776,15 +1780,18 @@
       <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="H5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" s="41" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1797,13 +1804,13 @@
       <c r="F6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="52"/>
-    </row>
-    <row r="7" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="9" t="s">
         <v>54</v>
       </c>
@@ -1816,30 +1823,31 @@
       <c r="F7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="52"/>
-    </row>
-    <row r="8" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="J7" s="41"/>
+    </row>
+    <row r="8" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="H9" s="44" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="H9" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="I9" s="24"/>
+      <c r="J9" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="38"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1852,15 +1860,18 @@
       <c r="F10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="H10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="40" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1873,13 +1884,13 @@
       <c r="F11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="51"/>
-    </row>
-    <row r="12" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="J11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="4" t="s">
         <v>54</v>
       </c>
@@ -1892,13 +1903,13 @@
       <c r="F12" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="51"/>
-    </row>
-    <row r="13" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="J12" s="40"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="4" t="s">
         <v>54</v>
       </c>
@@ -1911,13 +1922,13 @@
       <c r="F13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="50"/>
-    </row>
-    <row r="14" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="J13" s="28"/>
+    </row>
+    <row r="14" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
@@ -1931,11 +1942,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="9" t="s">
         <v>67</v>
       </c>
@@ -1948,30 +1959,30 @@
       <c r="F15" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="53"/>
-    </row>
-    <row r="16" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I16" s="53"/>
-    </row>
-    <row r="17" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
       <c r="H17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="53"/>
-    </row>
-    <row r="18" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1984,13 +1995,13 @@
       <c r="F18" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="53"/>
-    </row>
-    <row r="19" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="4" t="s">
         <v>49</v>
       </c>
@@ -2004,11 +2015,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+    <row r="20" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="4" t="s">
         <v>54</v>
       </c>
@@ -2022,11 +2033,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="39" t="s">
+    <row r="21" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="40"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="9" t="s">
         <v>49</v>
       </c>
@@ -2040,25 +2051,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+    <row r="22" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="48"/>
       <c r="H23" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+    <row r="24" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="4" t="s">
         <v>46</v>
       </c>
@@ -2072,11 +2083,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+    <row r="25" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="38"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="4" t="s">
         <v>49</v>
       </c>
@@ -2090,11 +2101,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
@@ -2108,11 +2119,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="4" t="s">
         <v>54</v>
       </c>
@@ -2126,11 +2137,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+    <row r="28" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="4" t="s">
         <v>49</v>
       </c>
@@ -2144,11 +2155,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+    <row r="29" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="4" t="s">
         <v>85</v>
       </c>
@@ -2162,11 +2173,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="39" t="s">
+    <row r="30" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="9" t="s">
         <v>85</v>
       </c>
@@ -2180,25 +2191,25 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+    <row r="31" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="48"/>
       <c r="H32" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
@@ -2212,11 +2223,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
+    <row r="34" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="4" t="s">
         <v>54</v>
       </c>
@@ -2230,11 +2241,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
+    <row r="35" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="4" t="s">
         <v>54</v>
       </c>
@@ -2248,11 +2259,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37" t="s">
+    <row r="36" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="4" t="s">
         <v>54</v>
       </c>
@@ -2266,11 +2277,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37" t="s">
+    <row r="37" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="4" t="s">
         <v>54</v>
       </c>
@@ -2284,11 +2295,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+    <row r="38" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="38"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="4" t="s">
         <v>67</v>
       </c>
@@ -2302,11 +2313,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+    <row r="39" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2320,11 +2331,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+    <row r="40" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="45"/>
       <c r="C40" s="4" t="s">
         <v>49</v>
       </c>
@@ -2338,11 +2349,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37" t="s">
+    <row r="41" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="38"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="4" t="s">
         <v>54</v>
       </c>
@@ -2356,7 +2367,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>135</v>
       </c>
@@ -2374,11 +2385,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37" t="s">
+    <row r="43" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="38"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="4" t="s">
         <v>49</v>
       </c>
@@ -2392,11 +2403,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+    <row r="44" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="4" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2421,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>145</v>
       </c>
@@ -2428,8 +2439,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="48" t="s">
+    <row r="46" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>146</v>
       </c>
       <c r="B46" s="4"/>
@@ -2446,11 +2457,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37" t="s">
+    <row r="47" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="4" t="s">
         <v>54</v>
       </c>
@@ -2464,11 +2475,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
+    <row r="48" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="38"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="4" t="s">
         <v>54</v>
       </c>
@@ -2482,11 +2493,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="37" t="s">
+    <row r="49" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="38"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="4" t="s">
         <v>54</v>
       </c>
@@ -2500,11 +2511,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="39" t="s">
+    <row r="50" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="40"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="9" t="s">
         <v>54</v>
       </c>
@@ -2518,25 +2529,25 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="41" t="s">
+    <row r="51" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="43"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="48"/>
       <c r="H52" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="37" t="s">
+    <row r="53" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="38"/>
+      <c r="B53" s="45"/>
       <c r="C53" s="4" t="s">
         <v>46</v>
       </c>
@@ -2550,11 +2561,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
+    <row r="54" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="38"/>
+      <c r="B54" s="45"/>
       <c r="C54" s="4" t="s">
         <v>49</v>
       </c>
@@ -2568,11 +2579,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="37" t="s">
+    <row r="55" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="38"/>
+      <c r="B55" s="45"/>
       <c r="C55" s="4" t="s">
         <v>54</v>
       </c>
@@ -2586,11 +2597,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
+    <row r="56" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="38"/>
+      <c r="B56" s="45"/>
       <c r="C56" s="4" t="s">
         <v>54</v>
       </c>
@@ -2604,11 +2615,11 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="37" t="s">
+    <row r="57" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="38"/>
+      <c r="B57" s="45"/>
       <c r="C57" s="4" t="s">
         <v>49</v>
       </c>
@@ -2622,11 +2633,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
+    <row r="58" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="38"/>
+      <c r="B58" s="45"/>
       <c r="C58" s="4" t="s">
         <v>49</v>
       </c>
@@ -2640,11 +2651,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="39" t="s">
+    <row r="59" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="40"/>
+      <c r="B59" s="43"/>
       <c r="C59" s="9" t="s">
         <v>49</v>
       </c>
@@ -2658,25 +2669,25 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="41" t="s">
+    <row r="60" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="43"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="48"/>
       <c r="H61" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
+    <row r="62" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B62" s="38"/>
+      <c r="B62" s="45"/>
       <c r="C62" s="4" t="s">
         <v>46</v>
       </c>
@@ -2690,11 +2701,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="37" t="s">
+    <row r="63" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="38"/>
+      <c r="B63" s="45"/>
       <c r="C63" s="4" t="s">
         <v>49</v>
       </c>
@@ -2708,11 +2719,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
+    <row r="64" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="38"/>
+      <c r="B64" s="45"/>
       <c r="C64" s="4" t="s">
         <v>49</v>
       </c>
@@ -2726,11 +2737,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45" t="s">
+    <row r="65" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="46"/>
+      <c r="B65" s="50"/>
       <c r="C65" s="6" t="s">
         <v>85</v>
       </c>
@@ -2740,15 +2751,15 @@
       <c r="E65" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F65" s="47" t="s">
+      <c r="F65" s="25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="39" t="s">
+    <row r="66" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="B66" s="40"/>
+      <c r="B66" s="43"/>
       <c r="C66" s="9" t="s">
         <v>85</v>
       </c>
@@ -2762,25 +2773,25 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
+    <row r="67" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B68" s="42"/>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="43"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="48"/>
       <c r="H68" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="37" t="s">
+    <row r="69" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="38"/>
+      <c r="B69" s="45"/>
       <c r="C69" s="4" t="s">
         <v>46</v>
       </c>
@@ -2794,11 +2805,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="37" t="s">
+    <row r="70" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="38"/>
+      <c r="B70" s="45"/>
       <c r="C70" s="4" t="s">
         <v>49</v>
       </c>
@@ -2812,11 +2823,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="37" t="s">
+    <row r="71" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B71" s="38"/>
+      <c r="B71" s="45"/>
       <c r="C71" s="4" t="s">
         <v>49</v>
       </c>
@@ -2830,11 +2841,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="37" t="s">
+    <row r="72" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="B72" s="38"/>
+      <c r="B72" s="45"/>
       <c r="C72" s="4" t="s">
         <v>126</v>
       </c>
@@ -2848,11 +2859,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="39" t="s">
+    <row r="73" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="40"/>
+      <c r="B73" s="43"/>
       <c r="C73" s="9" t="s">
         <v>49</v>
       </c>
@@ -2866,25 +2877,25 @@
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="41" t="s">
+    <row r="74" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="42"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42"/>
-      <c r="F75" s="43"/>
+      <c r="B75" s="47"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="48"/>
       <c r="H75" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="37" t="s">
+    <row r="76" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="38"/>
+      <c r="B76" s="45"/>
       <c r="C76" s="4" t="s">
         <v>46</v>
       </c>
@@ -2898,11 +2909,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="37" t="s">
+    <row r="77" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B77" s="38"/>
+      <c r="B77" s="45"/>
       <c r="C77" s="4" t="s">
         <v>49</v>
       </c>
@@ -2916,11 +2927,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="39" t="s">
+    <row r="78" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B78" s="40"/>
+      <c r="B78" s="43"/>
       <c r="C78" s="9" t="s">
         <v>49</v>
       </c>
@@ -2934,25 +2945,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="41" t="s">
+    <row r="79" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
-      <c r="F80" s="43"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="47"/>
+      <c r="E80" s="47"/>
+      <c r="F80" s="48"/>
       <c r="H80" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="37" t="s">
+    <row r="81" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="38"/>
+      <c r="B81" s="45"/>
       <c r="C81" s="4" t="s">
         <v>46</v>
       </c>
@@ -2966,11 +2977,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="37" t="s">
+    <row r="82" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="38"/>
+      <c r="B82" s="45"/>
       <c r="C82" s="4" t="s">
         <v>49</v>
       </c>
@@ -2984,11 +2995,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="39" t="s">
+    <row r="83" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B83" s="40"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="9" t="s">
         <v>49</v>
       </c>
@@ -3002,25 +3013,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="41" t="s">
+    <row r="84" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B85" s="42"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
-      <c r="F85" s="43"/>
+      <c r="B85" s="47"/>
+      <c r="C85" s="47"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="48"/>
       <c r="H85" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="37" t="s">
+    <row r="86" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="38"/>
+      <c r="B86" s="45"/>
       <c r="C86" s="4" t="s">
         <v>46</v>
       </c>
@@ -3034,11 +3045,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="37" t="s">
+    <row r="87" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="38"/>
+      <c r="B87" s="45"/>
       <c r="C87" s="4" t="s">
         <v>49</v>
       </c>
@@ -3052,11 +3063,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="39" t="s">
+    <row r="88" spans="1:8" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B88" s="40"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="9" t="s">
         <v>49</v>
       </c>
@@ -3072,65 +3083,6 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A86:B86"/>
@@ -3147,6 +3099,65 @@
     <mergeCell ref="A85:F85"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>